<commit_message>
Various improvements, inc (1) login using details from spreadsheet (2) scheduled runs using scheduler.py
</commit_message>
<xml_diff>
--- a/eric_data.xlsx
+++ b/eric_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25155" windowHeight="7080" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27525" windowHeight="6810" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenario" sheetId="1" r:id="rId1"/>
@@ -20,15 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="55">
   <si>
     <t>Test Scenario Setup</t>
   </si>
   <si>
-    <t>Spreadsheet used by spreadsheet_run.py</t>
-  </si>
-  <si>
-    <t>Gathers response times from Eric</t>
+    <t>Spreadsheet used by spreadsheet_run.py. Gathers response times from Eric.</t>
+  </si>
+  <si>
+    <t>Steps and data used in run</t>
   </si>
   <si>
     <t>Action</t>
@@ -61,7 +61,7 @@
     <t>All times in seconds</t>
   </si>
   <si>
-    <t>write results from row:</t>
+    <t>write next run to row:</t>
   </si>
   <si>
     <t>Run Start</t>
@@ -73,63 +73,72 @@
     <t>Search</t>
   </si>
   <si>
+    <t>Civil Financial Statement</t>
+  </si>
+  <si>
+    <t>Criminal Financial Statement</t>
+  </si>
+  <si>
+    <t>Mediation Financial Statement</t>
+  </si>
+  <si>
+    <t>Financial Statement Summary</t>
+  </si>
+  <si>
+    <t>Date/Time</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Select Time</t>
+  </si>
+  <si>
+    <t>Name Found</t>
+  </si>
+  <si>
+    <t>View Time</t>
+  </si>
+  <si>
+    <t>13/01/2018 - 09:21:01</t>
+  </si>
+  <si>
+    <t>0g934m</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Civil financial statement</t>
   </si>
   <si>
+    <t>2</t>
+  </si>
+  <si>
     <t>Criminal financial statement</t>
   </si>
   <si>
-    <t>Mediation financial statement</t>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Family mediation financial statement</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
   <si>
     <t>Financial statement summary</t>
   </si>
   <si>
-    <t>Date/Time</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>Position</t>
-  </si>
-  <si>
-    <t>Select Time</t>
-  </si>
-  <si>
-    <t>Name Found</t>
-  </si>
-  <si>
-    <t>View Time</t>
-  </si>
-  <si>
-    <t>13/01/2018 - 09:21:01</t>
-  </si>
-  <si>
-    <t>0g934m</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Family mediation financial statement</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>15/01/2018 - 09:04:50</t>
   </si>
   <si>
@@ -143,13 +152,46 @@
   </si>
   <si>
     <t>15/01/2018 - 09:33:08</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 12:00:04</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 12:14:19</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 12:22:51</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 12:26:41</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 12:30:42</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 12:35:02</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 12:36:34</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 14:50:19</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 14:51:45</t>
+  </si>
+  <si>
+    <t>Login Failed</t>
+  </si>
+  <si>
+    <t>15/01/2018 - 14:53:13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -195,6 +237,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
+      <name val="Liberation Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Liberation Sans"/>
       <family val="2"/>
     </font>
@@ -255,7 +310,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -391,20 +446,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -415,30 +506,68 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="2"/>
+    <cellStyle name="Heading" xfId="3"/>
     <cellStyle name="Heading1" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Result" xfId="3"/>
+    <cellStyle name="Result" xfId="2"/>
     <cellStyle name="Result2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -717,111 +846,119 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="26.875" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="23" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="30" t="s">
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="B11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="7"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="30" t="s">
+      <c r="B13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="30" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -831,29 +968,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="27" style="16" customWidth="1"/>
-    <col min="3" max="3" width="12" style="16" customWidth="1"/>
-    <col min="4" max="4" width="8.875" style="16" customWidth="1"/>
-    <col min="5" max="5" width="11.75" style="16" customWidth="1"/>
-    <col min="6" max="6" width="8.75" style="16" customWidth="1"/>
-    <col min="7" max="7" width="11.75" style="16" customWidth="1"/>
-    <col min="8" max="8" width="13.125" style="16" customWidth="1"/>
-    <col min="9" max="9" width="11.125" style="16" customWidth="1"/>
-    <col min="10" max="10" width="8.875" style="16" customWidth="1"/>
-    <col min="11" max="11" width="11.875" style="16" customWidth="1"/>
-    <col min="12" max="12" width="13.125" style="16" customWidth="1"/>
-    <col min="13" max="13" width="11.5" style="16" customWidth="1"/>
-    <col min="14" max="14" width="8" style="16" customWidth="1"/>
-    <col min="18" max="18" width="8.375" style="16" customWidth="1"/>
+    <col min="1" max="1" width="18.875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27" style="12" customWidth="1"/>
+    <col min="3" max="3" width="12" style="12" customWidth="1"/>
+    <col min="4" max="4" width="8.875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="12" customWidth="1"/>
+    <col min="6" max="6" width="8.75" style="30" customWidth="1"/>
+    <col min="7" max="7" width="11.75" style="12" customWidth="1"/>
+    <col min="8" max="8" width="13.125" style="12" customWidth="1"/>
+    <col min="9" max="9" width="11.125" style="12" customWidth="1"/>
+    <col min="10" max="10" width="8.875" style="30" customWidth="1"/>
+    <col min="11" max="11" width="11.875" style="12" customWidth="1"/>
+    <col min="12" max="12" width="13.125" style="12" customWidth="1"/>
+    <col min="13" max="13" width="11.5" style="12" customWidth="1"/>
+    <col min="14" max="14" width="8" style="30" customWidth="1"/>
+    <col min="18" max="18" width="8.375" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
@@ -862,118 +999,118 @@
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+      <c r="B3" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="U3" s="22"/>
+      <c r="C3" s="45">
+        <v>22</v>
+      </c>
+      <c r="U3" s="17"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="18" t="s">
+      <c r="E4" s="10"/>
+      <c r="F4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="23" t="s">
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="21"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="24" t="s">
+      <c r="K4" s="15"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="23" t="s">
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="S4" s="20"/>
-      <c r="T4" s="21"/>
-      <c r="U4" s="19"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="14"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="14" t="s">
+      <c r="N5" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="P5" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="Q5" s="14" t="s">
+      <c r="Q5" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="R5" s="15" t="s">
+      <c r="R5" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="S5" s="15" t="s">
+      <c r="S5" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="15" t="s">
+      <c r="T5" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="U5" s="15" t="s">
+      <c r="U5" s="43" t="s">
         <v>28</v>
       </c>
     </row>
@@ -984,437 +1121,1006 @@
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="19">
         <v>3.7300000190734859</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="19">
         <v>3.151000022888184</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="19">
         <v>3.151000022888184</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I6" s="27">
+        <v>32</v>
+      </c>
+      <c r="I6" s="20">
         <v>3.4489998817443852</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K6" s="26">
+      <c r="J6" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="19">
         <v>3.151000022888184</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M6" s="29">
+        <v>34</v>
+      </c>
+      <c r="M6" s="22">
         <v>3.4159998893737789</v>
       </c>
-      <c r="N6" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" s="28">
+      <c r="N6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O6" s="21">
         <v>3.151000022888184</v>
       </c>
-      <c r="P6" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="28">
+      <c r="P6" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" s="21">
         <v>3.2030000686645508</v>
       </c>
-      <c r="R6" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="S6" s="28">
+      <c r="R6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S6" s="21">
         <v>3.151000022888184</v>
       </c>
-      <c r="T6" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="U6" s="28">
+      <c r="T6" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U6" s="21">
         <v>3.3050000667572021</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="19">
         <v>4.2139999866485596</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="19">
         <v>3.1170001029968262</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="19">
         <v>3.1170001029968262</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="27">
+        <v>32</v>
+      </c>
+      <c r="I7" s="20">
         <v>3.720999956130981</v>
       </c>
-      <c r="J7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="26">
+      <c r="J7" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="19">
         <v>3.1170001029968262</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M7" s="29">
+        <v>34</v>
+      </c>
+      <c r="M7" s="22">
         <v>3.3789999485015869</v>
       </c>
-      <c r="N7" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O7" s="28">
+      <c r="N7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O7" s="21">
         <v>3.1170001029968262</v>
       </c>
-      <c r="P7" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="28">
+      <c r="P7" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q7" s="21">
         <v>3.1110000610351558</v>
       </c>
-      <c r="R7" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="28">
+      <c r="R7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" s="21">
         <v>3.1170001029968262</v>
       </c>
-      <c r="T7" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="U7" s="28">
+      <c r="T7" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" s="21">
         <v>3.288000106811523</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="19">
         <v>4.0439999103546143</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="19">
         <v>3.1400001049041748</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="19">
         <v>3.1400001049041748</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="27">
+        <v>32</v>
+      </c>
+      <c r="I8" s="20">
         <v>4.0369999408721924</v>
       </c>
-      <c r="J8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="26">
+      <c r="J8" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="19">
         <v>3.1400001049041748</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" s="29">
+        <v>34</v>
+      </c>
+      <c r="M8" s="22">
         <v>3.3869998455047612</v>
       </c>
-      <c r="N8" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O8" s="28">
+      <c r="N8" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O8" s="21">
         <v>3.1400001049041748</v>
       </c>
-      <c r="P8" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q8" s="28">
+      <c r="P8" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q8" s="21">
         <v>3.2060000896453862</v>
       </c>
-      <c r="R8" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="S8" s="28">
+      <c r="R8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S8" s="21">
         <v>3.1400001049041748</v>
       </c>
-      <c r="T8" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="28">
+      <c r="T8" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U8" s="21">
         <v>3.3240001201629639</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="19">
         <v>4.1619999408721924</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="19">
         <v>3.1129999160766602</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="19">
         <v>3.1129999160766602</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="27">
+        <v>32</v>
+      </c>
+      <c r="I9" s="20">
         <v>3.6730000972747798</v>
       </c>
-      <c r="J9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="26">
+      <c r="J9" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="19">
         <v>3.1129999160766602</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="29">
+        <v>34</v>
+      </c>
+      <c r="M9" s="22">
         <v>3.4790000915527339</v>
       </c>
-      <c r="N9" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O9" s="28">
+      <c r="N9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O9" s="21">
         <v>3.1129999160766602</v>
       </c>
-      <c r="P9" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q9" s="28">
+      <c r="P9" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" s="21">
         <v>3.1960000991821289</v>
       </c>
-      <c r="R9" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="S9" s="28">
+      <c r="R9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S9" s="21">
         <v>3.1129999160766602</v>
       </c>
-      <c r="T9" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="U9" s="28">
+      <c r="T9" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="21">
         <v>3.375</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="19">
         <v>4.8190000057220459</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="26">
+      <c r="E10" s="19">
         <v>3.184999942779541</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="19">
         <v>3.184999942779541</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="27">
+        <v>32</v>
+      </c>
+      <c r="I10" s="20">
         <v>3.5809998512268071</v>
       </c>
-      <c r="J10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" s="26">
+      <c r="J10" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="19">
         <v>3.184999942779541</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="29">
+        <v>34</v>
+      </c>
+      <c r="M10" s="22">
         <v>3.4309999942779541</v>
       </c>
-      <c r="N10" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="O10" s="28">
+      <c r="N10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="21">
         <v>3.184999942779541</v>
       </c>
-      <c r="P10" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q10" s="28">
+      <c r="P10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q10" s="21">
         <v>3.1690001487731929</v>
       </c>
-      <c r="R10" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="S10" s="28">
+      <c r="R10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S10" s="21">
         <v>3.184999942779541</v>
       </c>
-      <c r="T10" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="U10" s="28">
+      <c r="T10" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U10" s="21">
         <v>3.4240000247955318</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="19">
         <v>3.619999885559082</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="26">
+      <c r="E11" s="19">
         <v>3.1640000343322749</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="G11" s="26">
+      <c r="G11" s="19">
         <v>3.1640000343322749</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="27">
+        <v>32</v>
+      </c>
+      <c r="I11" s="20">
         <v>3.5119998455047612</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="19">
+        <v>3.1640000343322749</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="22">
+        <v>3.407999992370605</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O11" s="21">
+        <v>3.1640000343322749</v>
+      </c>
+      <c r="P11" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>3.3640000820159912</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S11" s="21">
+        <v>3.1640000343322749</v>
+      </c>
+      <c r="T11" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U11" s="21">
+        <v>3.3050000667572021</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="19">
+        <v>4.0739998817443848</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="19">
+        <v>3.1329998970031738</v>
+      </c>
+      <c r="F12" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="19">
+        <v>3.1329998970031738</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="26">
-        <v>3.1640000343322749</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="29">
-        <v>3.407999992370605</v>
-      </c>
-      <c r="N11" s="30" t="s">
+      <c r="I12" s="20">
+        <v>3.7079999446868901</v>
+      </c>
+      <c r="J12" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="28">
-        <v>3.1640000343322749</v>
-      </c>
-      <c r="P11" s="30" t="s">
+      <c r="K12" s="19">
+        <v>3.1329998970031738</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q11" s="28">
-        <v>3.3640000820159912</v>
-      </c>
-      <c r="R11" s="30" t="s">
+      <c r="M12" s="22">
+        <v>3.83899998664856</v>
+      </c>
+      <c r="N12" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="S11" s="28">
-        <v>3.1640000343322749</v>
-      </c>
-      <c r="T11" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="U11" s="28">
+      <c r="O12" s="21">
+        <v>3.1329998970031738</v>
+      </c>
+      <c r="P12" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>3.2920000553131099</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="S12" s="21">
+        <v>3.1329998970031738</v>
+      </c>
+      <c r="T12" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U12" s="21">
+        <v>3.278000116348267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="25">
+        <v>3.654000043869019</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="25">
+        <v>3.1159999370574951</v>
+      </c>
+      <c r="F13" s="33">
+        <v>1</v>
+      </c>
+      <c r="G13" s="25">
+        <v>3.1159999370574951</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="26">
+        <v>4.4570000171661377</v>
+      </c>
+      <c r="J13" s="33">
+        <v>2</v>
+      </c>
+      <c r="K13" s="25">
+        <v>3.1159999370574951</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="27">
+        <v>3.3940000534057622</v>
+      </c>
+      <c r="N13" s="36">
+        <v>3</v>
+      </c>
+      <c r="O13" s="29">
+        <v>3.1159999370574951</v>
+      </c>
+      <c r="P13" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q13" s="29">
+        <v>3.1960000991821289</v>
+      </c>
+      <c r="R13" s="36">
+        <v>4</v>
+      </c>
+      <c r="S13" s="29">
+        <v>3.1159999370574951</v>
+      </c>
+      <c r="T13" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="U13" s="29">
+        <v>3.5149998664855961</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="21">
+        <v>3.8949999809265141</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="21">
+        <v>3.1480000019073491</v>
+      </c>
+      <c r="F14" s="6">
+        <v>1</v>
+      </c>
+      <c r="G14" s="21">
+        <v>3.1480000019073491</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" s="21">
+        <v>3.5529999732971191</v>
+      </c>
+      <c r="J14" s="6">
+        <v>2</v>
+      </c>
+      <c r="K14" s="21">
+        <v>3.1480000019073491</v>
+      </c>
+      <c r="L14" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="21">
+        <v>3.407000064849854</v>
+      </c>
+      <c r="N14" s="6">
+        <v>3</v>
+      </c>
+      <c r="O14" s="21">
+        <v>3.1480000019073491</v>
+      </c>
+      <c r="P14" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>3.1110000610351558</v>
+      </c>
+      <c r="R14" s="6">
+        <v>4</v>
+      </c>
+      <c r="S14" s="21">
+        <v>3.1480000019073491</v>
+      </c>
+      <c r="T14" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U14" s="21">
         <v>3.3050000667572021</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="30"/>
-      <c r="O12" s="28"/>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="28"/>
-      <c r="R12" s="30"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="30"/>
-      <c r="U12" s="28"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="29"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="30"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="30"/>
-      <c r="U13" s="28"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="21">
+        <v>3.8619999885559082</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="21">
+        <v>3.1380000114440918</v>
+      </c>
+      <c r="F15" s="6">
+        <v>1</v>
+      </c>
+      <c r="G15" s="21">
+        <v>3.1380000114440918</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I15" s="21">
+        <v>3.6819999217987061</v>
+      </c>
+      <c r="J15" s="6">
+        <v>2</v>
+      </c>
+      <c r="K15" s="21">
+        <v>3.1380000114440918</v>
+      </c>
+      <c r="L15" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="21">
+        <v>3.342999935150146</v>
+      </c>
+      <c r="N15" s="6">
+        <v>3</v>
+      </c>
+      <c r="O15" s="21">
+        <v>3.1380000114440918</v>
+      </c>
+      <c r="P15" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>3.1669998168945308</v>
+      </c>
+      <c r="R15" s="6">
+        <v>4</v>
+      </c>
+      <c r="S15" s="21">
+        <v>3.1380000114440918</v>
+      </c>
+      <c r="T15" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U15" s="21">
+        <v>3.3220000267028809</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="21">
+        <v>3.8540000915527339</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="21">
+        <v>3.184999942779541</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1</v>
+      </c>
+      <c r="G16" s="21">
+        <v>3.184999942779541</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="21">
+        <v>3.5789999961853032</v>
+      </c>
+      <c r="J16" s="6">
+        <v>2</v>
+      </c>
+      <c r="K16" s="21">
+        <v>3.184999942779541</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="21">
+        <v>3.3859999179840088</v>
+      </c>
+      <c r="N16" s="6">
+        <v>3</v>
+      </c>
+      <c r="O16" s="21">
+        <v>3.184999942779541</v>
+      </c>
+      <c r="P16" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>3.1819999217987061</v>
+      </c>
+      <c r="R16" s="6">
+        <v>4</v>
+      </c>
+      <c r="S16" s="21">
+        <v>3.184999942779541</v>
+      </c>
+      <c r="T16" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U16" s="21">
+        <v>3.278999805450439</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="21">
+        <v>4.2630000114440918</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="21">
+        <v>3.2750000953674321</v>
+      </c>
+      <c r="F17" s="6">
+        <v>1</v>
+      </c>
+      <c r="G17" s="21">
+        <v>3.2750000953674321</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I17" s="21">
+        <v>3.7330000400543208</v>
+      </c>
+      <c r="J17" s="6">
+        <v>2</v>
+      </c>
+      <c r="K17" s="21">
+        <v>3.2750000953674321</v>
+      </c>
+      <c r="L17" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="21">
+        <v>3.3619999885559082</v>
+      </c>
+      <c r="N17" s="6">
+        <v>3</v>
+      </c>
+      <c r="O17" s="21">
+        <v>3.2750000953674321</v>
+      </c>
+      <c r="P17" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>3.3299999237060551</v>
+      </c>
+      <c r="R17" s="6">
+        <v>4</v>
+      </c>
+      <c r="S17" s="21">
+        <v>3.2750000953674321</v>
+      </c>
+      <c r="T17" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U17" s="21">
+        <v>3.280999898910522</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="21">
+        <v>3.7199997901916499</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="21">
+        <v>3.1119999885559082</v>
+      </c>
+      <c r="F18" s="6">
+        <v>1</v>
+      </c>
+      <c r="G18" s="21">
+        <v>3.1119999885559082</v>
+      </c>
+      <c r="H18" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I18" s="21">
+        <v>3.601000070571899</v>
+      </c>
+      <c r="J18" s="6">
+        <v>2</v>
+      </c>
+      <c r="K18" s="21">
+        <v>3.1119999885559082</v>
+      </c>
+      <c r="L18" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="21">
+        <v>3.2679998874664311</v>
+      </c>
+      <c r="N18" s="6">
+        <v>3</v>
+      </c>
+      <c r="O18" s="21">
+        <v>3.1119999885559082</v>
+      </c>
+      <c r="P18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>3.192000150680542</v>
+      </c>
+      <c r="R18" s="6">
+        <v>4</v>
+      </c>
+      <c r="S18" s="21">
+        <v>3.1119999885559082</v>
+      </c>
+      <c r="T18" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U18" s="21">
+        <v>3.280999898910522</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="21">
+        <v>4.0659999847412109</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="21">
+        <v>3.127000093460083</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="21">
+        <v>3.127000093460083</v>
+      </c>
+      <c r="H19" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I19" s="21">
+        <v>3.5850000381469731</v>
+      </c>
+      <c r="J19" s="6">
+        <v>2</v>
+      </c>
+      <c r="K19" s="21">
+        <v>3.127000093460083</v>
+      </c>
+      <c r="L19" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" s="21">
+        <v>3.4099998474121089</v>
+      </c>
+      <c r="N19" s="6">
+        <v>3</v>
+      </c>
+      <c r="O19" s="21">
+        <v>3.127000093460083</v>
+      </c>
+      <c r="P19" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>3.246999979019165</v>
+      </c>
+      <c r="R19" s="6">
+        <v>4</v>
+      </c>
+      <c r="S19" s="21">
+        <v>3.127000093460083</v>
+      </c>
+      <c r="T19" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U19" s="21">
+        <v>3.3020000457763672</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D20" s="23"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="23"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="23"/>
+      <c r="U20" s="21"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="21">
+        <v>3.7950000762939449</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="21">
+        <v>3.1269998550415039</v>
+      </c>
+      <c r="F21" s="6">
+        <v>1</v>
+      </c>
+      <c r="G21" s="21">
+        <v>3.1269998550415039</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" s="21">
+        <v>3.6059999465942378</v>
+      </c>
+      <c r="J21" s="6">
+        <v>2</v>
+      </c>
+      <c r="K21" s="21">
+        <v>3.1269998550415039</v>
+      </c>
+      <c r="L21" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" s="21">
+        <v>3.3209998607635498</v>
+      </c>
+      <c r="N21" s="6">
+        <v>3</v>
+      </c>
+      <c r="O21" s="21">
+        <v>3.1269998550415039</v>
+      </c>
+      <c r="P21" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>3.1779999732971191</v>
+      </c>
+      <c r="R21" s="6">
+        <v>4</v>
+      </c>
+      <c r="S21" s="21">
+        <v>3.1269998550415039</v>
+      </c>
+      <c r="T21" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="U21" s="21">
+        <v>3.307999849319458</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000Page &amp;P</oddFooter>

</xml_diff>